<commit_message>
Added instagram extraction code; reading json works and text is outputted to console; now have to show it properly on screen
</commit_message>
<xml_diff>
--- a/csv/data.xlsx
+++ b/csv/data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shrut\Desktop\projects\WhatsTrendingInGeorgiaTech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juilee Rege\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF29180E-32A1-4347-8336-F715B28FA149}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8210" xr2:uid="{6AEFB085-5136-4352-84D3-D65215146723}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t xml:space="preserve">Page Name </t>
   </si>
@@ -136,9 +135,6 @@
   </si>
   <si>
     <t>Instagram</t>
-  </si>
-  <si>
-    <t>@GTFBRecruiting</t>
   </si>
   <si>
     <t>@GTAthletics</t>
@@ -431,52 +427,34 @@
     <t>Georgia Tech India Club is one of the largest student cultural organizations at Georgia Tech and in the South East. Follow us to learn more!</t>
   </si>
   <si>
-    <t>georgiatech</t>
-  </si>
-  <si>
-    <t>sppgatech</t>
-  </si>
-  <si>
-    <t>gtcomputing</t>
-  </si>
-  <si>
-    <t>gatechengineers</t>
-  </si>
-  <si>
-    <t>gtalumni</t>
-  </si>
-  <si>
-    <t>gtwbb</t>
-  </si>
-  <si>
-    <t>#gtmbb</t>
-  </si>
-  <si>
-    <t>georgiatechfb</t>
-  </si>
-  <si>
-    <t>gtathletics</t>
-  </si>
-  <si>
-    <t>gt_baseball</t>
-  </si>
-  <si>
-    <t>gt_wten</t>
-  </si>
-  <si>
-    <t>gt_mten</t>
-  </si>
-  <si>
-    <t>gatechsoftball</t>
-  </si>
-  <si>
-    <t>gt_tracknfield</t>
+    <t>#georgiatechfb</t>
+  </si>
+  <si>
+    <t>#georgiatechgolf</t>
+  </si>
+  <si>
+    <t>#gt_baseball</t>
+  </si>
+  <si>
+    <t>#georgiatechathletics</t>
+  </si>
+  <si>
+    <t>#georgiatechsoftball</t>
+  </si>
+  <si>
+    <t>#georgiatechtrackandfield</t>
+  </si>
+  <si>
+    <t>#georgiatechband</t>
+  </si>
+  <si>
+    <t>#georgiatechresearchinstitute</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -512,11 +490,10 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF262626"/>
-      <name val="Segoe UI"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -556,9 +533,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -873,22 +848,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0205CEAD-97CE-4263-AF46-3DAD09182435}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="92.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="92.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,21 +874,18 @@
         <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="25" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -921,7 +893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -929,7 +901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -937,7 +909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -945,7 +917,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -953,7 +925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -961,29 +933,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -991,41 +957,38 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="25" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -1033,494 +996,485 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="25" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="25" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="C22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="25" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="4" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="25" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="4" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="25" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="25" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="1" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="4" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="D35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+      <c r="B36" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="4" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="4" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+      <c r="B39" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="B40" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
+      <c r="B42" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="5" t="s">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
+      <c r="B43" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="4" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
+      <c r="B44" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="4" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="4" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="4" t="s">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+      <c r="B56" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="4" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
+      <c r="B57" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="4" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
+      <c r="B60" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B60" s="4" t="s">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+      <c r="B62" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="4" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
+      <c r="B63" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="4" t="s">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="1" t="s">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B65" s="1" t="s">
+    </row>
+    <row r="66" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" s="6" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="25" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B66" s="4" t="s">
+      <c r="D66" t="s">
         <v>127</v>
       </c>
-      <c r="C66" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D66" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
+      <c r="B67" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://twitter.com/GeorgiaTech" xr:uid="{3AB0C321-5280-401B-AAF4-15BE5D01D3AA}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://twitter.com/gtbuzztap" xr:uid="{6CF625CD-7500-4FCC-9977-41530851256A}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://twitter.com/GT_Sciences" xr:uid="{F2EB2350-4F3C-43C8-B2B1-B2587AF80D46}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://twitter.com/GTPhysics" xr:uid="{F0119B01-9AF5-499C-B871-CB8D8EA97C04}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://twitter.com/GATechEcon" xr:uid="{18E5A036-901F-41E5-A167-8BDF9C0878DE}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://twitter.com/GTliberalarts" xr:uid="{37829D55-B618-4A4F-BD5C-2006AE56C213}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://twitter.com/IvanAllenGT" xr:uid="{038A614C-7B68-46CF-AA64-AC1B022F54A2}"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://twitter.com/sppgatech" xr:uid="{9496F281-09FE-458B-BEC5-974B1D3C0914}"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://twitter.com/gtcomputing" xr:uid="{40864818-B824-4846-94BA-889456D25013}"/>
-    <hyperlink ref="A11" r:id="rId10" display="https://twitter.com/GeorgiaTech_ECE" xr:uid="{4B1E9A06-0E6E-42EF-9349-075D32F54CC7}"/>
-    <hyperlink ref="A12" r:id="rId11" display="https://twitter.com/GTRI" xr:uid="{DE55F27F-397B-45A8-85A4-F60AC2DA68F6}"/>
-    <hyperlink ref="A13" r:id="rId12" display="https://twitter.com/GaTechEngineers" xr:uid="{0A2A0091-91AA-409D-A239-9A9C46C0D488}"/>
-    <hyperlink ref="A14" r:id="rId13" display="https://twitter.com/gtalumni" xr:uid="{8541E5F9-FDF9-4EF3-BA5E-C4DC6D5FD9DF}"/>
-    <hyperlink ref="A16" r:id="rId14" display="https://twitter.com/GTStudents" xr:uid="{932C54BD-BEEA-4142-A871-27F9593DF832}"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://twitter.com/gtstudents" xr:uid="{8DFD4384-1DCB-4FA0-8032-1F5AB23F87AB}"/>
-    <hyperlink ref="A18" r:id="rId16" display="https://twitter.com/GTMBB" xr:uid="{FC6C5F00-0B7F-4B8D-A107-EF2A8C9F97A2}"/>
-    <hyperlink ref="C20" r:id="rId17" display="https://twitter.com/GTFBRecruiting" xr:uid="{EC0B1AC4-5AD3-422E-8A04-0FDA6F6B09B7}"/>
-    <hyperlink ref="A21" r:id="rId18" display="https://twitter.com/GTAthletics" xr:uid="{6E3AA4C2-2636-443C-BA4C-C8D3D7A8D83C}"/>
-    <hyperlink ref="A22" r:id="rId19" display="https://twitter.com/GTBaseball" xr:uid="{2991BC05-D44D-45DA-BE04-8C37F45E5C91}"/>
-    <hyperlink ref="A23" r:id="rId20" display="https://twitter.com/GT_WTEN" xr:uid="{6C04C8D9-DFBA-4707-9FA3-9D257E5E2D72}"/>
-    <hyperlink ref="A24" r:id="rId21" display="https://twitter.com/GT_MTEN" xr:uid="{EFAB5B05-2D2A-415C-B31D-95EB30E4B7DF}"/>
-    <hyperlink ref="A25" r:id="rId22" display="https://twitter.com/GaTechSoftball" xr:uid="{45DEAFE5-D59D-4E17-8ACC-A50ED6098296}"/>
-    <hyperlink ref="A17" r:id="rId23" display="https://twitter.com/GTWBB" xr:uid="{8DF80302-C8B2-48C5-B976-E4F678A75139}"/>
-    <hyperlink ref="A26" r:id="rId24" display="https://twitter.com/GT_trackNfield" xr:uid="{8EEE5AA8-013F-4368-933F-58CEF7999737}"/>
-    <hyperlink ref="A28" r:id="rId25" display="https://twitter.com/GeorgiaTechBand" xr:uid="{87007149-D55B-4331-B0DF-9A01C24178F4}"/>
-    <hyperlink ref="A29" r:id="rId26" display="https://twitter.com/GTCheerleading" xr:uid="{2E783902-1BA7-4046-9A4B-637196263047}"/>
-    <hyperlink ref="C29" r:id="rId27" display="https://twitter.com/gtcheerleading" xr:uid="{FAC85AB8-FECC-43CE-AEFD-057C9D23B87B}"/>
-    <hyperlink ref="A30" r:id="rId28" display="https://twitter.com/GTGoldrush" xr:uid="{E41B038A-DCB7-4EDD-B156-4B81333A964A}"/>
-    <hyperlink ref="C30" r:id="rId29" display="https://twitter.com/gtgoldrush" xr:uid="{A66AF118-C798-4A78-BEE7-9C2CC0556D68}"/>
-    <hyperlink ref="A32" r:id="rId30" display="https://twitter.com/Buzz_GT" xr:uid="{6FD003A3-8CEB-4A5D-BE12-E5E0EED72424}"/>
-    <hyperlink ref="A33" r:id="rId31" display="https://twitter.com/GeorgiaTechMBA" xr:uid="{038196A7-B13C-4632-AEFB-A44744203D40}"/>
-    <hyperlink ref="A34" r:id="rId32" display="https://twitter.com/georgiatechbsch" xr:uid="{A74680B9-64AD-41B0-B659-E071E1CF8A7A}"/>
-    <hyperlink ref="B34" r:id="rId33" display="https://twitter.com/GeorgiaTech" xr:uid="{4BC41AA3-0EBC-4553-93B8-E67EF004BF52}"/>
-    <hyperlink ref="A35" r:id="rId34" display="https://twitter.com/GatechEsports" xr:uid="{6C4B2269-932B-4F4C-B9F2-1B17E9980BB5}"/>
-    <hyperlink ref="A36" r:id="rId35" display="https://twitter.com/GTTribe" xr:uid="{2B1A8963-7C52-415F-B6DC-F54D54B1A9F0}"/>
-    <hyperlink ref="A37" r:id="rId36" display="https://twitter.com/GaTech_Hotel" xr:uid="{64B702EF-0E1E-4564-A727-E8B5D1CACCE1}"/>
-    <hyperlink ref="A38" r:id="rId37" display="https://twitter.com/GTDining" xr:uid="{E995B82A-1F41-4435-A38D-8A67331E9E95}"/>
-    <hyperlink ref="A39" r:id="rId38" display="https://twitter.com/GTClough" xr:uid="{36F7D248-CD61-4F2E-92D8-C7C138CDD149}"/>
-    <hyperlink ref="A40" r:id="rId39" display="https://twitter.com/GTLibrary" xr:uid="{BB5CCF8E-AA2F-4CD2-96F3-B93F78AEE73A}"/>
-    <hyperlink ref="A41" r:id="rId40" display="https://twitter.com/gt_park_trans" xr:uid="{1D70EAFB-28E5-49D1-A197-F9BF0921753F}"/>
-    <hyperlink ref="A42" r:id="rId41" display="https://twitter.com/Gatechoit" xr:uid="{7F189D08-86BA-41FE-B976-4AE27B71E9BB}"/>
-    <hyperlink ref="A43" r:id="rId42" display="https://twitter.com/GTaerospace" xr:uid="{829B78A5-4E35-4F34-A3C3-B706BB17BD4C}"/>
-    <hyperlink ref="A44" r:id="rId43" display="https://twitter.com/MEGeorgiaTech" xr:uid="{4166CD7C-D9D3-4682-96D2-F34092E4FD7B}"/>
-    <hyperlink ref="A45" r:id="rId44" display="https://twitter.com/GaTechPD" xr:uid="{540CBE08-E888-4B9C-8F16-04161FF4963A}"/>
-    <hyperlink ref="A46" r:id="rId45" display="https://twitter.com/GTPDalerts" xr:uid="{4EB8381F-36D1-4B28-800D-B8C2457E1B7F}"/>
-    <hyperlink ref="A47" r:id="rId46" display="https://twitter.com/TechHSOC" xr:uid="{9BA15847-7623-4D83-8758-68932F7F6FEC}"/>
-    <hyperlink ref="A52" r:id="rId47" display="https://twitter.com/GTSAA" xr:uid="{F3B184A1-912C-423D-BAE8-F94476B1652B}"/>
-    <hyperlink ref="A53" r:id="rId48" display="https://twitter.com/GATechBookstore" xr:uid="{6BEB8B4F-BA78-4280-95C7-9D2FA617681E}"/>
-    <hyperlink ref="A54" r:id="rId49" display="https://twitter.com/gatechsga" xr:uid="{27F8AF77-3A33-4248-8FDE-A68987A37CE7}"/>
-    <hyperlink ref="A55" r:id="rId50" display="https://twitter.com/GTOMSCS" xr:uid="{5EEA43F2-AA32-4DF7-A8F2-74B8559F9273}"/>
-    <hyperlink ref="A56" r:id="rId51" display="https://twitter.com/CRCatGT" xr:uid="{F633B42E-13B5-4981-A273-AD747BD5334A}"/>
-    <hyperlink ref="A57" r:id="rId52" display="https://twitter.com/HealthyGT" xr:uid="{7FD53303-0C6E-4252-876F-CD811D90D620}"/>
-    <hyperlink ref="A58" r:id="rId53" display="https://twitter.com/GaTechHousing" xr:uid="{6FC8916B-FFD4-4057-B932-9B3A4EC776B7}"/>
-    <hyperlink ref="A59" r:id="rId54" display="https://twitter.com/GaTechLEAD" xr:uid="{AEBD5EA0-1130-4C1B-83ED-5C3BCB5B0634}"/>
-    <hyperlink ref="A60" r:id="rId55" display="https://twitter.com/GTNSTP" xr:uid="{FAC5856F-C9B1-4D58-AAA7-DDD0DDFF2E24}"/>
-    <hyperlink ref="A61" r:id="rId56" display="https://twitter.com/GT_Facilities" xr:uid="{7CB8D65E-1111-435D-8D92-6D6EB48624C0}"/>
-    <hyperlink ref="A62" r:id="rId57" display="https://twitter.com/GTCounseling" xr:uid="{8B1FA2B8-5BB9-4CE1-8888-2D9E7121E047}"/>
-    <hyperlink ref="A63" r:id="rId58" display="https://twitter.com/GT_CHEM" xr:uid="{628C8982-B30A-476D-998C-98F53751D17D}"/>
-    <hyperlink ref="A64" r:id="rId59" display="https://twitter.com/GTStudentCenter" xr:uid="{CFF373EE-98C2-4FE2-9B7A-57307C1115F8}"/>
-    <hyperlink ref="A65" r:id="rId60" display="https://twitter.com/GATECH_DesignIT" xr:uid="{659DD449-363A-41E8-89C1-9CED98644EC2}"/>
-    <hyperlink ref="A66" r:id="rId61" display="https://twitter.com/TEDxGeorgiaTech" xr:uid="{7F4F14D5-2E51-41E0-A246-BCC3F8E21B20}"/>
-    <hyperlink ref="A67" r:id="rId62" display="https://twitter.com/GTIndiaClub" xr:uid="{46C3D646-7101-42BA-80A6-EDA0BFF074EC}"/>
-    <hyperlink ref="A27" r:id="rId63" display="https://twitter.com/GT_GOLF" xr:uid="{23966AFC-C2FB-42CC-AA8D-7411F0B0B336}"/>
-    <hyperlink ref="A20" r:id="rId64" display="https://twitter.com/GTFootball" xr:uid="{EC624DEF-EA2F-44BE-8136-F6BAE6CEFE14}"/>
-    <hyperlink ref="A19" r:id="rId65" display="https://twitter.com/GeorgiaTechFB" xr:uid="{B2A472D0-E7C6-48EF-83D6-056EE8BA3963}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://twitter.com/GeorgiaTech"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://twitter.com/gtbuzztap"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://twitter.com/GT_Sciences"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://twitter.com/GTPhysics"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://twitter.com/GATechEcon"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://twitter.com/GTliberalarts"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://twitter.com/IvanAllenGT"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://twitter.com/sppgatech"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://twitter.com/gtcomputing"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://twitter.com/GeorgiaTech_ECE"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://twitter.com/GTRI"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://twitter.com/GaTechEngineers"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://twitter.com/gtalumni"/>
+    <hyperlink ref="A16" r:id="rId14" display="https://twitter.com/GTStudents"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://twitter.com/gtstudents"/>
+    <hyperlink ref="A18" r:id="rId16" display="https://twitter.com/GTMBB"/>
+    <hyperlink ref="A19" r:id="rId17" display="https://twitter.com/GeorgiaTechFB"/>
+    <hyperlink ref="A20" r:id="rId18" display="https://twitter.com/GTFootball"/>
+    <hyperlink ref="C19" r:id="rId19" display="https://twitter.com/GTFBRecruiting"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://twitter.com/GTAthletics"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://twitter.com/GTBaseball"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://twitter.com/GT_WTEN"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://twitter.com/GT_MTEN"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://twitter.com/GaTechSoftball"/>
+    <hyperlink ref="A17" r:id="rId25" display="https://twitter.com/GTWBB"/>
+    <hyperlink ref="A26" r:id="rId26" display="https://twitter.com/GT_trackNfield"/>
+    <hyperlink ref="A27" r:id="rId27" display="https://twitter.com/GT_GOLF"/>
+    <hyperlink ref="A28" r:id="rId28" display="https://twitter.com/GeorgiaTechBand"/>
+    <hyperlink ref="A29" r:id="rId29" display="https://twitter.com/GTCheerleading"/>
+    <hyperlink ref="A30" r:id="rId30" display="https://twitter.com/GTGoldrush"/>
+    <hyperlink ref="C30" r:id="rId31" display="https://twitter.com/gtgoldrush"/>
+    <hyperlink ref="A32" r:id="rId32" display="https://twitter.com/Buzz_GT"/>
+    <hyperlink ref="A33" r:id="rId33" display="https://twitter.com/GeorgiaTechMBA"/>
+    <hyperlink ref="A34" r:id="rId34" display="https://twitter.com/georgiatechbsch"/>
+    <hyperlink ref="B34" r:id="rId35" display="https://twitter.com/GeorgiaTech"/>
+    <hyperlink ref="A35" r:id="rId36" display="https://twitter.com/GatechEsports"/>
+    <hyperlink ref="A36" r:id="rId37" display="https://twitter.com/GTTribe"/>
+    <hyperlink ref="A37" r:id="rId38" display="https://twitter.com/GaTech_Hotel"/>
+    <hyperlink ref="A38" r:id="rId39" display="https://twitter.com/GTDining"/>
+    <hyperlink ref="A39" r:id="rId40" display="https://twitter.com/GTClough"/>
+    <hyperlink ref="A40" r:id="rId41" display="https://twitter.com/GTLibrary"/>
+    <hyperlink ref="A41" r:id="rId42" display="https://twitter.com/gt_park_trans"/>
+    <hyperlink ref="A42" r:id="rId43" display="https://twitter.com/Gatechoit"/>
+    <hyperlink ref="A43" r:id="rId44" display="https://twitter.com/GTaerospace"/>
+    <hyperlink ref="A44" r:id="rId45" display="https://twitter.com/MEGeorgiaTech"/>
+    <hyperlink ref="A45" r:id="rId46" display="https://twitter.com/GaTechPD"/>
+    <hyperlink ref="A46" r:id="rId47" display="https://twitter.com/GTPDalerts"/>
+    <hyperlink ref="A47" r:id="rId48" display="https://twitter.com/TechHSOC"/>
+    <hyperlink ref="A52" r:id="rId49" display="https://twitter.com/GTSAA"/>
+    <hyperlink ref="A53" r:id="rId50" display="https://twitter.com/GATechBookstore"/>
+    <hyperlink ref="A54" r:id="rId51" display="https://twitter.com/gatechsga"/>
+    <hyperlink ref="A55" r:id="rId52" display="https://twitter.com/GTOMSCS"/>
+    <hyperlink ref="A56" r:id="rId53" display="https://twitter.com/CRCatGT"/>
+    <hyperlink ref="A57" r:id="rId54" display="https://twitter.com/HealthyGT"/>
+    <hyperlink ref="A58" r:id="rId55" display="https://twitter.com/GaTechHousing"/>
+    <hyperlink ref="A59" r:id="rId56" display="https://twitter.com/GaTechLEAD"/>
+    <hyperlink ref="A60" r:id="rId57" display="https://twitter.com/GTNSTP"/>
+    <hyperlink ref="A61" r:id="rId58" display="https://twitter.com/GT_Facilities"/>
+    <hyperlink ref="A62" r:id="rId59" display="https://twitter.com/GTCounseling"/>
+    <hyperlink ref="A63" r:id="rId60" display="https://twitter.com/GT_CHEM"/>
+    <hyperlink ref="A64" r:id="rId61" display="https://twitter.com/GTStudentCenter"/>
+    <hyperlink ref="A65" r:id="rId62" display="https://twitter.com/GATECH_DesignIT"/>
+    <hyperlink ref="A66" r:id="rId63" display="https://twitter.com/TEDxGeorgiaTech"/>
+    <hyperlink ref="A67" r:id="rId64" display="https://twitter.com/GTIndiaClub"/>
+    <hyperlink ref="C29" r:id="rId65" display="https://twitter.com/gtcheerleading"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId66"/>

</xml_diff>